<commit_message>
formenschlüssel extrahiert, prozesse teilweise extrahiert
</commit_message>
<xml_diff>
--- a/datenRF4/AFL/i=23,28 Scheibenbremse, Abtriebswelle=14/Prozesse_Stückliste_L1_S4_i23,28_Scheiben.xlsx
+++ b/datenRF4/AFL/i=23,28 Scheibenbremse, Abtriebswelle=14/Prozesse_Stückliste_L1_S4_i23,28_Scheiben.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_11A2CD86AE0A81C8BF9B0D8C1CF59A0A403392D0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_C290A855DAC40C962C62F7F11F9DD7CB5330F6B8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="142">
   <si>
     <t>Benennung:</t>
   </si>
@@ -1212,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1335,9 +1335,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
@@ -1446,6 +1443,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1496,7 +1502,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1802,18 +1808,18 @@
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="130"/>
-      <c r="J1" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="132"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1">
       <c r="A2" s="21" t="s">
@@ -3725,18 +3731,18 @@
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="130"/>
-      <c r="J1" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="132"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1">
       <c r="A2" s="21" t="s">
@@ -5681,18 +5687,18 @@
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="130"/>
-      <c r="J1" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="132"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1">
       <c r="A2" s="21" t="s">
@@ -7637,18 +7643,18 @@
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
-      <c r="F1" s="127" t="s">
+      <c r="F1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="130"/>
-      <c r="J1" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="132"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="132"/>
+      <c r="J1" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1">
       <c r="A2" s="21" t="s">
@@ -9571,8 +9577,8 @@
   <dimension ref="A1:U340"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="I94" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E108" sqref="E108:G108"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -9584,7 +9590,7 @@
     <col min="4" max="4" width="4.5703125" customWidth="1"/>
     <col min="5" max="5" width="31.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="114" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="113" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
@@ -9597,7 +9603,7 @@
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" customWidth="1"/>
     <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="123" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="122" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.85546875" customWidth="1"/>
     <col min="23" max="23" width="13.85546875" customWidth="1"/>
@@ -9607,60 +9613,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="141" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="143" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="141"/>
-      <c r="K1" s="141"/>
-      <c r="L1" s="141"/>
-      <c r="M1" s="133" t="s">
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="135" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
-      <c r="P1" s="133"/>
-      <c r="Q1" s="133"/>
-      <c r="R1" s="133"/>
-      <c r="S1" s="133"/>
-      <c r="T1" s="133"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="135"/>
+      <c r="R1" s="135"/>
+      <c r="S1" s="135"/>
+      <c r="T1" s="135"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="136"/>
-      <c r="C2" s="137" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="138"/>
-      <c r="E2" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="140"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="133"/>
-      <c r="O2" s="133"/>
-      <c r="P2" s="133"/>
-      <c r="Q2" s="133"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="133"/>
-      <c r="T2" s="133"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="139" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="140"/>
+      <c r="E2" s="141" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="142"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="135"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1">
       <c r="A3" s="69" t="s">
@@ -9678,10 +9684,10 @@
       <c r="E3" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="94" t="s">
+      <c r="F3" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="114" t="s">
         <v>135</v>
       </c>
       <c r="H3" s="71" t="s">
@@ -9720,7 +9726,7 @@
       <c r="S3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="118" t="s">
+      <c r="T3" s="117" t="s">
         <v>18</v>
       </c>
     </row>
@@ -9730,8 +9736,8 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="104"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="29">
         <v>0</v>
       </c>
@@ -9756,7 +9762,7 @@
       <c r="S4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="119"/>
+      <c r="T4" s="118"/>
     </row>
     <row r="5" spans="1:20" ht="15" thickBot="1">
       <c r="A5" s="75"/>
@@ -9765,7 +9771,7 @@
       <c r="D5" s="73"/>
       <c r="E5" s="73"/>
       <c r="F5" s="73"/>
-      <c r="G5" s="124"/>
+      <c r="G5" s="123"/>
       <c r="H5" s="29">
         <v>1</v>
       </c>
@@ -9786,7 +9792,7 @@
         <v>26</v>
       </c>
       <c r="S5" s="29"/>
-      <c r="T5" s="120"/>
+      <c r="T5" s="119"/>
     </row>
     <row r="6" spans="1:20" ht="72.599999999999994">
       <c r="A6" s="5">
@@ -9804,10 +9810,10 @@
       <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="104"/>
+      <c r="G6" s="103"/>
       <c r="H6" s="29">
         <v>2</v>
       </c>
@@ -9836,7 +9842,7 @@
       <c r="S6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="120">
+      <c r="T6" s="119">
         <v>1</v>
       </c>
     </row>
@@ -9853,13 +9859,13 @@
       <c r="D7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="105"/>
+      <c r="G7" s="104"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
@@ -9872,26 +9878,28 @@
       <c r="Q7" s="29"/>
       <c r="R7" s="29"/>
       <c r="S7" s="29"/>
-      <c r="T7" s="120"/>
+      <c r="T7" s="119"/>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1">
       <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="77"/>
+      <c r="B8" s="126">
+        <v>3</v>
+      </c>
       <c r="C8" s="24">
         <v>1</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="102">
+      <c r="G8" s="101">
         <v>23255</v>
       </c>
       <c r="H8" s="29"/>
@@ -9906,7 +9914,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
       <c r="S8" s="29"/>
-      <c r="T8" s="120"/>
+      <c r="T8" s="119"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="30"/>
@@ -9915,7 +9923,7 @@
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
-      <c r="G9" s="124"/>
+      <c r="G9" s="123"/>
       <c r="H9" s="29">
         <v>2</v>
       </c>
@@ -9933,7 +9941,7 @@
       <c r="Q9" s="29"/>
       <c r="R9" s="29"/>
       <c r="S9" s="29"/>
-      <c r="T9" s="120"/>
+      <c r="T9" s="119"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="30"/>
@@ -9942,7 +9950,7 @@
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
-      <c r="G10" s="124"/>
+      <c r="G10" s="123"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
@@ -9957,7 +9965,7 @@
       <c r="Q10" s="29"/>
       <c r="R10" s="29"/>
       <c r="S10" s="29"/>
-      <c r="T10" s="120"/>
+      <c r="T10" s="119"/>
     </row>
     <row r="11" spans="1:20" ht="15" thickBot="1">
       <c r="A11" s="30"/>
@@ -9966,7 +9974,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="124"/>
+      <c r="G11" s="123"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
@@ -9979,7 +9987,7 @@
       <c r="Q11" s="29"/>
       <c r="R11" s="29"/>
       <c r="S11" s="29"/>
-      <c r="T11" s="120"/>
+      <c r="T11" s="119"/>
     </row>
     <row r="12" spans="1:20" ht="72.599999999999994">
       <c r="A12" s="5">
@@ -10000,7 +10008,7 @@
       <c r="F12" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="104"/>
+      <c r="G12" s="103"/>
       <c r="H12" s="29">
         <v>3</v>
       </c>
@@ -10029,7 +10037,7 @@
       <c r="S12" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="120">
+      <c r="T12" s="119">
         <v>1</v>
       </c>
     </row>
@@ -10046,13 +10054,13 @@
       <c r="D13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="81" t="s">
+      <c r="E13" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="85" t="s">
+      <c r="F13" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="106"/>
+      <c r="G13" s="105"/>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
@@ -10065,26 +10073,28 @@
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
       <c r="S13" s="29"/>
-      <c r="T13" s="120"/>
+      <c r="T13" s="119"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="79">
-        <v>1</v>
-      </c>
-      <c r="B14" s="32"/>
+      <c r="A14" s="78">
+        <v>1</v>
+      </c>
+      <c r="B14" s="127">
+        <v>3</v>
+      </c>
       <c r="C14" s="28">
         <v>1</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="87" t="s">
+      <c r="F14" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="99">
+      <c r="G14" s="98">
         <v>23255</v>
       </c>
       <c r="H14" s="29"/>
@@ -10099,13 +10109,15 @@
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
       <c r="S14" s="29"/>
-      <c r="T14" s="120"/>
+      <c r="T14" s="119"/>
     </row>
     <row r="15" spans="1:20" ht="15" thickBot="1">
       <c r="A15" s="13">
         <v>2</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="128">
+        <v>3</v>
+      </c>
       <c r="C15" s="15">
         <v>1</v>
       </c>
@@ -10118,7 +10130,7 @@
       <c r="F15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="100">
+      <c r="G15" s="99">
         <v>16102</v>
       </c>
       <c r="H15" s="29"/>
@@ -10133,7 +10145,7 @@
       <c r="Q15" s="29"/>
       <c r="R15" s="29"/>
       <c r="S15" s="29"/>
-      <c r="T15" s="120"/>
+      <c r="T15" s="119"/>
     </row>
     <row r="16" spans="1:20" ht="72.599999999999994">
       <c r="A16" s="30"/>
@@ -10142,7 +10154,7 @@
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
-      <c r="G16" s="124"/>
+      <c r="G16" s="123"/>
       <c r="H16" s="29">
         <v>4</v>
       </c>
@@ -10163,7 +10175,7 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="120"/>
+      <c r="T16" s="119"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="30"/>
@@ -10172,7 +10184,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="124"/>
+      <c r="G17" s="123"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -10185,7 +10197,7 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
       <c r="S17" s="29"/>
-      <c r="T17" s="120"/>
+      <c r="T17" s="119"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="30"/>
@@ -10194,7 +10206,7 @@
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="124"/>
+      <c r="G18" s="123"/>
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
@@ -10207,7 +10219,7 @@
       <c r="Q18" s="29"/>
       <c r="R18" s="29"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="120"/>
+      <c r="T18" s="119"/>
     </row>
     <row r="19" spans="1:20" ht="15" thickBot="1">
       <c r="A19" s="30"/>
@@ -10216,7 +10228,7 @@
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="124"/>
+      <c r="G19" s="123"/>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
@@ -10229,7 +10241,7 @@
       <c r="Q19" s="29"/>
       <c r="R19" s="29"/>
       <c r="S19" s="29"/>
-      <c r="T19" s="120"/>
+      <c r="T19" s="119"/>
     </row>
     <row r="20" spans="1:20" ht="72.599999999999994">
       <c r="A20" s="5">
@@ -10250,7 +10262,7 @@
       <c r="F20" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="104"/>
+      <c r="G20" s="103"/>
       <c r="H20" s="29">
         <v>5</v>
       </c>
@@ -10279,30 +10291,30 @@
       <c r="S20" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T20" s="120">
+      <c r="T20" s="119">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" thickBot="1">
-      <c r="A21" s="82">
-        <v>2</v>
-      </c>
-      <c r="B21" s="83">
-        <v>2</v>
-      </c>
-      <c r="C21" s="81">
-        <v>1</v>
-      </c>
-      <c r="D21" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="81" t="s">
+      <c r="A21" s="81">
+        <v>2</v>
+      </c>
+      <c r="B21" s="82">
+        <v>2</v>
+      </c>
+      <c r="C21" s="80">
+        <v>1</v>
+      </c>
+      <c r="D21" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="88" t="s">
+      <c r="F21" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="107"/>
+      <c r="G21" s="106"/>
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -10315,26 +10327,28 @@
       <c r="Q21" s="29"/>
       <c r="R21" s="29"/>
       <c r="S21" s="29"/>
-      <c r="T21" s="120"/>
+      <c r="T21" s="119"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="79">
-        <v>1</v>
-      </c>
-      <c r="B22" s="32"/>
+      <c r="A22" s="78">
+        <v>1</v>
+      </c>
+      <c r="B22" s="127">
+        <v>3</v>
+      </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="99">
+      <c r="G22" s="98">
         <v>22302</v>
       </c>
       <c r="H22" s="29"/>
@@ -10349,13 +10363,15 @@
       <c r="Q22" s="29"/>
       <c r="R22" s="29"/>
       <c r="S22" s="29"/>
-      <c r="T22" s="120"/>
+      <c r="T22" s="119"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="6">
         <v>2</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="127">
+        <v>3</v>
+      </c>
       <c r="C23" s="8">
         <v>1</v>
       </c>
@@ -10365,10 +10381,10 @@
       <c r="E23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="89" t="s">
+      <c r="F23" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="101">
+      <c r="G23" s="100">
         <v>20122</v>
       </c>
       <c r="H23" s="29"/>
@@ -10383,13 +10399,15 @@
       <c r="Q23" s="29"/>
       <c r="R23" s="29"/>
       <c r="S23" s="29"/>
-      <c r="T23" s="120"/>
+      <c r="T23" s="119"/>
     </row>
     <row r="24" spans="1:20" ht="29.45" thickBot="1">
       <c r="A24" s="13">
         <v>3</v>
       </c>
-      <c r="B24" s="14"/>
+      <c r="B24" s="128">
+        <v>3</v>
+      </c>
       <c r="C24" s="15">
         <v>8</v>
       </c>
@@ -10402,7 +10420,7 @@
       <c r="F24" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="100"/>
+      <c r="G24" s="99"/>
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
@@ -10415,7 +10433,7 @@
       <c r="Q24" s="29"/>
       <c r="R24" s="29"/>
       <c r="S24" s="29"/>
-      <c r="T24" s="120"/>
+      <c r="T24" s="119"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="30"/>
@@ -10424,7 +10442,7 @@
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="124"/>
+      <c r="G25" s="123"/>
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -10437,7 +10455,7 @@
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
       <c r="S25" s="29"/>
-      <c r="T25" s="120"/>
+      <c r="T25" s="119"/>
     </row>
     <row r="26" spans="1:20" ht="29.1">
       <c r="A26" s="30"/>
@@ -10446,7 +10464,7 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
-      <c r="G26" s="124"/>
+      <c r="G26" s="123"/>
       <c r="H26" s="29">
         <v>5</v>
       </c>
@@ -10467,7 +10485,7 @@
       <c r="Q26" s="29"/>
       <c r="R26" s="29"/>
       <c r="S26" s="29"/>
-      <c r="T26" s="120"/>
+      <c r="T26" s="119"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="30"/>
@@ -10476,7 +10494,7 @@
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="124"/>
+      <c r="G27" s="123"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
@@ -10489,7 +10507,7 @@
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
       <c r="S27" s="29"/>
-      <c r="T27" s="120"/>
+      <c r="T27" s="119"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="30"/>
@@ -10498,7 +10516,7 @@
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
-      <c r="G28" s="124"/>
+      <c r="G28" s="123"/>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
@@ -10511,7 +10529,7 @@
       <c r="Q28" s="29"/>
       <c r="R28" s="29"/>
       <c r="S28" s="29"/>
-      <c r="T28" s="120"/>
+      <c r="T28" s="119"/>
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="30"/>
@@ -10520,7 +10538,7 @@
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
-      <c r="G29" s="124"/>
+      <c r="G29" s="123"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
@@ -10533,7 +10551,7 @@
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
-      <c r="T29" s="120"/>
+      <c r="T29" s="119"/>
     </row>
     <row r="30" spans="1:20" ht="15" thickBot="1">
       <c r="A30" s="30"/>
@@ -10542,7 +10560,7 @@
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
-      <c r="G30" s="124"/>
+      <c r="G30" s="123"/>
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
@@ -10555,7 +10573,7 @@
       <c r="Q30" s="29"/>
       <c r="R30" s="29"/>
       <c r="S30" s="29"/>
-      <c r="T30" s="120"/>
+      <c r="T30" s="119"/>
     </row>
     <row r="31" spans="1:20" ht="72.599999999999994">
       <c r="A31" s="5">
@@ -10576,7 +10594,7 @@
       <c r="F31" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G31" s="104"/>
+      <c r="G31" s="103"/>
       <c r="H31" s="29">
         <v>6</v>
       </c>
@@ -10605,30 +10623,30 @@
       <c r="S31" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T31" s="120">
+      <c r="T31" s="119">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15" thickBot="1">
-      <c r="A32" s="82">
-        <v>2</v>
-      </c>
-      <c r="B32" s="83">
-        <v>2</v>
-      </c>
-      <c r="C32" s="81">
-        <v>1</v>
-      </c>
-      <c r="D32" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="81" t="s">
+      <c r="A32" s="81">
+        <v>2</v>
+      </c>
+      <c r="B32" s="82">
+        <v>2</v>
+      </c>
+      <c r="C32" s="80">
+        <v>1</v>
+      </c>
+      <c r="D32" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="88" t="s">
+      <c r="F32" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="107"/>
+      <c r="G32" s="106"/>
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
@@ -10641,26 +10659,28 @@
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
-      <c r="T32" s="120"/>
+      <c r="T32" s="119"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="79">
-        <v>1</v>
-      </c>
-      <c r="B33" s="32"/>
+      <c r="A33" s="78">
+        <v>1</v>
+      </c>
+      <c r="B33" s="127">
+        <v>3</v>
+      </c>
       <c r="C33" s="28">
         <v>1</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="80" t="s">
+      <c r="E33" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="87" t="s">
+      <c r="F33" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="99">
+      <c r="G33" s="98">
         <v>23255</v>
       </c>
       <c r="H33" s="29"/>
@@ -10675,13 +10695,15 @@
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
       <c r="S33" s="29"/>
-      <c r="T33" s="120"/>
+      <c r="T33" s="119"/>
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="6">
         <v>2</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="127">
+        <v>3</v>
+      </c>
       <c r="C34" s="8">
         <v>1</v>
       </c>
@@ -10691,10 +10713,10 @@
       <c r="E34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="89" t="s">
+      <c r="F34" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="101">
+      <c r="G34" s="100">
         <v>20122</v>
       </c>
       <c r="H34" s="29"/>
@@ -10709,13 +10731,15 @@
       <c r="Q34" s="29"/>
       <c r="R34" s="29"/>
       <c r="S34" s="29"/>
-      <c r="T34" s="120"/>
+      <c r="T34" s="119"/>
     </row>
     <row r="35" spans="1:20" ht="29.45" thickBot="1">
       <c r="A35" s="13">
         <v>3</v>
       </c>
-      <c r="B35" s="14"/>
+      <c r="B35" s="128">
+        <v>3</v>
+      </c>
       <c r="C35" s="15">
         <v>8</v>
       </c>
@@ -10728,7 +10752,7 @@
       <c r="F35" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="100"/>
+      <c r="G35" s="99"/>
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
       <c r="J35" s="29"/>
@@ -10741,7 +10765,7 @@
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
       <c r="S35" s="29"/>
-      <c r="T35" s="120"/>
+      <c r="T35" s="119"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="30"/>
@@ -10750,7 +10774,7 @@
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
-      <c r="G36" s="124"/>
+      <c r="G36" s="123"/>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
@@ -10763,7 +10787,7 @@
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
       <c r="S36" s="29"/>
-      <c r="T36" s="120"/>
+      <c r="T36" s="119"/>
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="30"/>
@@ -10772,7 +10796,7 @@
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
       <c r="F37" s="29"/>
-      <c r="G37" s="124"/>
+      <c r="G37" s="123"/>
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
@@ -10785,7 +10809,7 @@
       <c r="Q37" s="29"/>
       <c r="R37" s="29"/>
       <c r="S37" s="29"/>
-      <c r="T37" s="120"/>
+      <c r="T37" s="119"/>
     </row>
     <row r="38" spans="1:20" ht="29.1">
       <c r="A38" s="30"/>
@@ -10794,7 +10818,7 @@
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="124"/>
+      <c r="G38" s="123"/>
       <c r="H38" s="29">
         <v>6</v>
       </c>
@@ -10815,7 +10839,7 @@
       <c r="Q38" s="29"/>
       <c r="R38" s="29"/>
       <c r="S38" s="29"/>
-      <c r="T38" s="120"/>
+      <c r="T38" s="119"/>
     </row>
     <row r="39" spans="1:20">
       <c r="A39" s="30"/>
@@ -10824,7 +10848,7 @@
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
-      <c r="G39" s="124"/>
+      <c r="G39" s="123"/>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
@@ -10837,7 +10861,7 @@
       <c r="Q39" s="29"/>
       <c r="R39" s="29"/>
       <c r="S39" s="29"/>
-      <c r="T39" s="120"/>
+      <c r="T39" s="119"/>
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="30"/>
@@ -10846,7 +10870,7 @@
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
-      <c r="G40" s="124"/>
+      <c r="G40" s="123"/>
       <c r="H40" s="29"/>
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
@@ -10859,7 +10883,7 @@
       <c r="Q40" s="29"/>
       <c r="R40" s="29"/>
       <c r="S40" s="29"/>
-      <c r="T40" s="120"/>
+      <c r="T40" s="119"/>
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="30"/>
@@ -10868,7 +10892,7 @@
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
       <c r="F41" s="29"/>
-      <c r="G41" s="124"/>
+      <c r="G41" s="123"/>
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
       <c r="J41" s="29"/>
@@ -10881,7 +10905,7 @@
       <c r="Q41" s="29"/>
       <c r="R41" s="29"/>
       <c r="S41" s="29"/>
-      <c r="T41" s="120"/>
+      <c r="T41" s="119"/>
     </row>
     <row r="42" spans="1:20" ht="15" thickBot="1">
       <c r="A42" s="30"/>
@@ -10890,7 +10914,7 @@
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
-      <c r="G42" s="124"/>
+      <c r="G42" s="123"/>
       <c r="H42" s="29"/>
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
@@ -10903,7 +10927,7 @@
       <c r="Q42" s="29"/>
       <c r="R42" s="29"/>
       <c r="S42" s="29"/>
-      <c r="T42" s="120"/>
+      <c r="T42" s="119"/>
     </row>
     <row r="43" spans="1:20" ht="57.95">
       <c r="A43" s="5">
@@ -10924,7 +10948,7 @@
       <c r="F43" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G43" s="104"/>
+      <c r="G43" s="103"/>
       <c r="H43" s="29">
         <v>7</v>
       </c>
@@ -10957,28 +10981,28 @@
       <c r="S43" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="T43" s="120"/>
+      <c r="T43" s="119"/>
     </row>
     <row r="44" spans="1:20" ht="29.45" thickBot="1">
-      <c r="A44" s="82">
-        <v>2</v>
-      </c>
-      <c r="B44" s="83">
-        <v>2</v>
-      </c>
-      <c r="C44" s="81">
-        <v>1</v>
-      </c>
-      <c r="D44" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="81" t="s">
+      <c r="A44" s="81">
+        <v>2</v>
+      </c>
+      <c r="B44" s="82">
+        <v>2</v>
+      </c>
+      <c r="C44" s="80">
+        <v>1</v>
+      </c>
+      <c r="D44" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="F44" s="88" t="s">
+      <c r="F44" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="107"/>
+      <c r="G44" s="106"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
@@ -10997,26 +11021,28 @@
       <c r="S44" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="T44" s="120"/>
+      <c r="T44" s="119"/>
     </row>
     <row r="45" spans="1:20">
-      <c r="A45" s="79">
-        <v>1</v>
-      </c>
-      <c r="B45" s="32"/>
+      <c r="A45" s="78">
+        <v>1</v>
+      </c>
+      <c r="B45" s="127">
+        <v>3</v>
+      </c>
       <c r="C45" s="28">
         <v>1</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="80" t="s">
+      <c r="E45" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F45" s="87" t="s">
+      <c r="F45" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="99">
+      <c r="G45" s="98">
         <v>23255</v>
       </c>
       <c r="H45" s="29"/>
@@ -11031,13 +11057,15 @@
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="29"/>
-      <c r="T45" s="120"/>
+      <c r="T45" s="119"/>
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="6">
         <v>2</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="127">
+        <v>3</v>
+      </c>
       <c r="C46" s="8">
         <v>1</v>
       </c>
@@ -11047,10 +11075,10 @@
       <c r="E46" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="89" t="s">
+      <c r="F46" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="101">
+      <c r="G46" s="100">
         <v>20122</v>
       </c>
       <c r="H46" s="29"/>
@@ -11065,13 +11093,15 @@
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="120"/>
+      <c r="T46" s="119"/>
     </row>
     <row r="47" spans="1:20" ht="29.45" thickBot="1">
       <c r="A47" s="13">
         <v>3</v>
       </c>
-      <c r="B47" s="14"/>
+      <c r="B47" s="128">
+        <v>3</v>
+      </c>
       <c r="C47" s="15">
         <v>8</v>
       </c>
@@ -11084,7 +11114,7 @@
       <c r="F47" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G47" s="100">
+      <c r="G47" s="99">
         <v>16122</v>
       </c>
       <c r="H47" s="29"/>
@@ -11099,7 +11129,7 @@
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-      <c r="T47" s="120"/>
+      <c r="T47" s="119"/>
     </row>
     <row r="48" spans="1:20" ht="15" thickBot="1">
       <c r="A48" s="30"/>
@@ -11108,7 +11138,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
-      <c r="G48" s="124"/>
+      <c r="G48" s="123"/>
       <c r="H48" s="29">
         <v>7</v>
       </c>
@@ -11129,7 +11159,7 @@
       <c r="Q48" s="29"/>
       <c r="R48" s="29"/>
       <c r="S48" s="29"/>
-      <c r="T48" s="120"/>
+      <c r="T48" s="119"/>
     </row>
     <row r="49" spans="1:20" ht="72.599999999999994">
       <c r="A49" s="5">
@@ -11150,7 +11180,7 @@
       <c r="F49" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G49" s="104"/>
+      <c r="G49" s="103"/>
       <c r="H49" s="29">
         <v>8</v>
       </c>
@@ -11179,7 +11209,7 @@
       <c r="S49" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T49" s="120">
+      <c r="T49" s="119">
         <v>1</v>
       </c>
     </row>
@@ -11199,10 +11229,10 @@
       <c r="E50" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="90" t="s">
+      <c r="F50" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G50" s="108"/>
+      <c r="G50" s="107"/>
       <c r="H50" s="29"/>
       <c r="I50" s="29"/>
       <c r="J50" s="29"/>
@@ -11215,20 +11245,28 @@
       <c r="Q50" s="29"/>
       <c r="R50" s="29"/>
       <c r="S50" s="29"/>
-      <c r="T50" s="120"/>
+      <c r="T50" s="119"/>
     </row>
     <row r="51" spans="1:20" ht="15" thickBot="1">
-      <c r="A51" s="82"/>
-      <c r="B51" s="81"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81" t="s">
+      <c r="A51" s="81">
+        <v>3</v>
+      </c>
+      <c r="B51" s="82">
+        <v>2</v>
+      </c>
+      <c r="C51" s="8">
+        <v>1</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="F51" s="88" t="s">
+      <c r="F51" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="109"/>
+      <c r="G51" s="108"/>
       <c r="H51" s="29"/>
       <c r="I51" s="29"/>
       <c r="J51" s="29"/>
@@ -11241,20 +11279,28 @@
       <c r="Q51" s="29"/>
       <c r="R51" s="29"/>
       <c r="S51" s="29"/>
-      <c r="T51" s="120"/>
+      <c r="T51" s="119"/>
     </row>
     <row r="52" spans="1:20" ht="15" thickBot="1">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
+      <c r="A52" s="23">
+        <v>1</v>
+      </c>
+      <c r="B52" s="24">
+        <v>3</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E52" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="91" t="s">
+      <c r="F52" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="G52" s="110">
+      <c r="G52" s="109">
         <v>11322</v>
       </c>
       <c r="H52" s="29"/>
@@ -11269,7 +11315,7 @@
       <c r="Q52" s="29"/>
       <c r="R52" s="29"/>
       <c r="S52" s="29"/>
-      <c r="T52" s="120"/>
+      <c r="T52" s="119"/>
     </row>
     <row r="53" spans="1:20" ht="15" thickBot="1">
       <c r="A53" s="30"/>
@@ -11278,7 +11324,7 @@
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
       <c r="F53" s="29"/>
-      <c r="G53" s="125"/>
+      <c r="G53" s="124"/>
       <c r="H53" s="29"/>
       <c r="I53" s="29"/>
       <c r="J53" s="29"/>
@@ -11291,7 +11337,7 @@
       <c r="Q53" s="29"/>
       <c r="R53" s="29"/>
       <c r="S53" s="29"/>
-      <c r="T53" s="120"/>
+      <c r="T53" s="119"/>
     </row>
     <row r="54" spans="1:20" ht="72.599999999999994">
       <c r="A54" s="5">
@@ -11312,7 +11358,7 @@
       <c r="F54" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G54" s="104"/>
+      <c r="G54" s="103"/>
       <c r="H54" s="29">
         <v>9</v>
       </c>
@@ -11341,7 +11387,7 @@
       <c r="S54" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T54" s="120">
+      <c r="T54" s="119">
         <v>1</v>
       </c>
     </row>
@@ -11361,10 +11407,10 @@
       <c r="E55" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="90" t="s">
+      <c r="F55" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G55" s="108"/>
+      <c r="G55" s="107"/>
       <c r="H55" s="29"/>
       <c r="I55" s="29"/>
       <c r="J55" s="29"/>
@@ -11377,24 +11423,28 @@
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-      <c r="T55" s="120"/>
+      <c r="T55" s="119"/>
     </row>
     <row r="56" spans="1:20" ht="15" thickBot="1">
-      <c r="A56" s="82"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="81">
-        <v>1</v>
-      </c>
-      <c r="D56" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="81" t="s">
+      <c r="A56" s="81">
+        <v>3</v>
+      </c>
+      <c r="B56" s="82">
+        <v>2</v>
+      </c>
+      <c r="C56" s="80">
+        <v>1</v>
+      </c>
+      <c r="D56" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="88" t="s">
+      <c r="F56" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="107"/>
+      <c r="G56" s="106"/>
       <c r="H56" s="29"/>
       <c r="I56" s="29"/>
       <c r="J56" s="29"/>
@@ -11407,11 +11457,15 @@
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-      <c r="T56" s="120"/>
+      <c r="T56" s="119"/>
     </row>
     <row r="57" spans="1:20">
-      <c r="A57" s="79"/>
-      <c r="B57" s="28"/>
+      <c r="A57" s="78">
+        <v>1</v>
+      </c>
+      <c r="B57" s="28">
+        <v>3</v>
+      </c>
       <c r="C57" s="28">
         <v>1</v>
       </c>
@@ -11421,10 +11475,10 @@
       <c r="E57" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F57" s="92" t="s">
+      <c r="F57" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="G57" s="111">
+      <c r="G57" s="110">
         <v>11322</v>
       </c>
       <c r="H57" s="29"/>
@@ -11439,11 +11493,15 @@
       <c r="Q57" s="29"/>
       <c r="R57" s="29"/>
       <c r="S57" s="29"/>
-      <c r="T57" s="120"/>
+      <c r="T57" s="119"/>
     </row>
     <row r="58" spans="1:20" ht="15" thickBot="1">
-      <c r="A58" s="13"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="13">
+        <v>2</v>
+      </c>
+      <c r="B58" s="15">
+        <v>3</v>
+      </c>
       <c r="C58" s="74">
         <v>6</v>
       </c>
@@ -11453,10 +11511,10 @@
       <c r="E58" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F58" s="93" t="s">
+      <c r="F58" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="G58" s="112">
+      <c r="G58" s="111">
         <v>16122</v>
       </c>
       <c r="H58" s="29"/>
@@ -11471,7 +11529,7 @@
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="120"/>
+      <c r="T58" s="119"/>
     </row>
     <row r="59" spans="1:20" ht="15" thickBot="1">
       <c r="A59" s="30"/>
@@ -11480,7 +11538,7 @@
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
       <c r="F59" s="29"/>
-      <c r="G59" s="124"/>
+      <c r="G59" s="123"/>
       <c r="H59" s="29"/>
       <c r="I59" s="29"/>
       <c r="J59" s="29"/>
@@ -11493,7 +11551,7 @@
       <c r="Q59" s="29"/>
       <c r="R59" s="29"/>
       <c r="S59" s="29"/>
-      <c r="T59" s="120"/>
+      <c r="T59" s="119"/>
     </row>
     <row r="60" spans="1:20" ht="57.95">
       <c r="A60" s="5">
@@ -11514,7 +11572,7 @@
       <c r="F60" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G60" s="104"/>
+      <c r="G60" s="103"/>
       <c r="H60" s="29">
         <v>10</v>
       </c>
@@ -11547,7 +11605,7 @@
       <c r="S60" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="T60" s="120"/>
+      <c r="T60" s="119"/>
     </row>
     <row r="61" spans="1:20" ht="29.1">
       <c r="A61" s="6">
@@ -11565,10 +11623,10 @@
       <c r="E61" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F61" s="90" t="s">
+      <c r="F61" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G61" s="108"/>
+      <c r="G61" s="107"/>
       <c r="H61" s="29">
         <v>11</v>
       </c>
@@ -11595,24 +11653,28 @@
       <c r="S61" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="T61" s="120"/>
+      <c r="T61" s="119"/>
     </row>
     <row r="62" spans="1:20" ht="15" thickBot="1">
-      <c r="A62" s="82"/>
-      <c r="B62" s="81"/>
-      <c r="C62" s="81">
-        <v>1</v>
-      </c>
-      <c r="D62" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E62" s="81" t="s">
+      <c r="A62" s="81">
+        <v>3</v>
+      </c>
+      <c r="B62" s="82">
+        <v>2</v>
+      </c>
+      <c r="C62" s="80">
+        <v>1</v>
+      </c>
+      <c r="D62" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E62" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="F62" s="88" t="s">
+      <c r="F62" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="107"/>
+      <c r="G62" s="106"/>
       <c r="H62" s="29"/>
       <c r="I62" s="29"/>
       <c r="J62" s="29"/>
@@ -11625,11 +11687,15 @@
       <c r="Q62" s="29"/>
       <c r="R62" s="29"/>
       <c r="S62" s="29"/>
-      <c r="T62" s="120"/>
+      <c r="T62" s="119"/>
     </row>
     <row r="63" spans="1:20">
-      <c r="A63" s="79"/>
-      <c r="B63" s="28"/>
+      <c r="A63" s="78">
+        <v>1</v>
+      </c>
+      <c r="B63" s="28">
+        <v>3</v>
+      </c>
       <c r="C63" s="28">
         <v>1</v>
       </c>
@@ -11639,10 +11705,10 @@
       <c r="E63" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F63" s="92" t="s">
+      <c r="F63" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="G63" s="111">
+      <c r="G63" s="110">
         <v>11322</v>
       </c>
       <c r="H63" s="29"/>
@@ -11657,11 +11723,15 @@
       <c r="Q63" s="29"/>
       <c r="R63" s="29"/>
       <c r="S63" s="29"/>
-      <c r="T63" s="120"/>
+      <c r="T63" s="119"/>
     </row>
     <row r="64" spans="1:20" ht="15" thickBot="1">
-      <c r="A64" s="13"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="13">
+        <v>2</v>
+      </c>
+      <c r="B64" s="15">
+        <v>3</v>
+      </c>
       <c r="C64" s="74">
         <v>6</v>
       </c>
@@ -11671,10 +11741,10 @@
       <c r="E64" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F64" s="93" t="s">
+      <c r="F64" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="G64" s="112">
+      <c r="G64" s="111">
         <v>16122</v>
       </c>
       <c r="H64" s="29"/>
@@ -11689,7 +11759,7 @@
       <c r="Q64" s="29"/>
       <c r="R64" s="29"/>
       <c r="S64" s="29"/>
-      <c r="T64" s="120"/>
+      <c r="T64" s="119"/>
     </row>
     <row r="65" spans="1:20">
       <c r="A65" s="30"/>
@@ -11698,7 +11768,7 @@
       <c r="D65" s="29"/>
       <c r="E65" s="29"/>
       <c r="F65" s="29"/>
-      <c r="G65" s="124"/>
+      <c r="G65" s="123"/>
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
       <c r="J65" s="29"/>
@@ -11711,7 +11781,7 @@
       <c r="Q65" s="29"/>
       <c r="R65" s="29"/>
       <c r="S65" s="29"/>
-      <c r="T65" s="120"/>
+      <c r="T65" s="119"/>
     </row>
     <row r="66" spans="1:20" ht="43.5">
       <c r="A66" s="30"/>
@@ -11720,7 +11790,7 @@
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
       <c r="F66" s="29"/>
-      <c r="G66" s="124"/>
+      <c r="G66" s="123"/>
       <c r="H66" s="29">
         <v>12</v>
       </c>
@@ -11741,7 +11811,7 @@
       <c r="Q66" s="29"/>
       <c r="R66" s="29"/>
       <c r="S66" s="29"/>
-      <c r="T66" s="120"/>
+      <c r="T66" s="119"/>
     </row>
     <row r="67" spans="1:20" ht="43.5">
       <c r="A67" s="30"/>
@@ -11750,7 +11820,7 @@
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
       <c r="F67" s="29"/>
-      <c r="G67" s="124"/>
+      <c r="G67" s="123"/>
       <c r="H67" s="29">
         <v>12</v>
       </c>
@@ -11771,7 +11841,7 @@
       <c r="Q67" s="29"/>
       <c r="R67" s="29"/>
       <c r="S67" s="29"/>
-      <c r="T67" s="120"/>
+      <c r="T67" s="119"/>
     </row>
     <row r="68" spans="1:20" ht="43.5">
       <c r="A68" s="30"/>
@@ -11780,7 +11850,7 @@
       <c r="D68" s="29"/>
       <c r="E68" s="29"/>
       <c r="F68" s="29"/>
-      <c r="G68" s="124"/>
+      <c r="G68" s="123"/>
       <c r="H68" s="29">
         <v>12</v>
       </c>
@@ -11801,7 +11871,7 @@
       <c r="Q68" s="29"/>
       <c r="R68" s="29"/>
       <c r="S68" s="29"/>
-      <c r="T68" s="120"/>
+      <c r="T68" s="119"/>
     </row>
     <row r="69" spans="1:20" ht="44.1" thickBot="1">
       <c r="A69" s="30"/>
@@ -11810,7 +11880,7 @@
       <c r="D69" s="29"/>
       <c r="E69" s="29"/>
       <c r="F69" s="29"/>
-      <c r="G69" s="124"/>
+      <c r="G69" s="123"/>
       <c r="H69" s="29">
         <v>12</v>
       </c>
@@ -11831,7 +11901,7 @@
       <c r="Q69" s="29"/>
       <c r="R69" s="29"/>
       <c r="S69" s="29"/>
-      <c r="T69" s="120"/>
+      <c r="T69" s="119"/>
     </row>
     <row r="70" spans="1:20" ht="72.599999999999994">
       <c r="A70" s="5">
@@ -11852,7 +11922,7 @@
       <c r="F70" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G70" s="104"/>
+      <c r="G70" s="103"/>
       <c r="H70" s="29">
         <v>13</v>
       </c>
@@ -11881,7 +11951,7 @@
       <c r="S70" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T70" s="120">
+      <c r="T70" s="119">
         <v>1</v>
       </c>
     </row>
@@ -11901,10 +11971,10 @@
       <c r="E71" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="90" t="s">
+      <c r="F71" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G71" s="108"/>
+      <c r="G71" s="107"/>
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
       <c r="J71" s="29"/>
@@ -11917,20 +11987,28 @@
       <c r="Q71" s="29"/>
       <c r="R71" s="29"/>
       <c r="S71" s="29"/>
-      <c r="T71" s="120"/>
+      <c r="T71" s="119"/>
     </row>
     <row r="72" spans="1:20">
-      <c r="A72" s="6"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
+      <c r="A72" s="6">
+        <v>3</v>
+      </c>
+      <c r="B72" s="7">
+        <v>2</v>
+      </c>
+      <c r="C72" s="8">
+        <v>1</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E72" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F72" s="90" t="s">
+      <c r="F72" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="G72" s="108"/>
+      <c r="G72" s="107"/>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
@@ -11943,28 +12021,28 @@
       <c r="Q72" s="29"/>
       <c r="R72" s="29"/>
       <c r="S72" s="29"/>
-      <c r="T72" s="120"/>
+      <c r="T72" s="119"/>
     </row>
     <row r="73" spans="1:20" ht="15" thickBot="1">
-      <c r="A73" s="82">
-        <v>3</v>
-      </c>
-      <c r="B73" s="83">
-        <v>2</v>
-      </c>
-      <c r="C73" s="81">
-        <v>1</v>
-      </c>
-      <c r="D73" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E73" s="81" t="s">
+      <c r="A73" s="81">
+        <v>4</v>
+      </c>
+      <c r="B73" s="82">
+        <v>2</v>
+      </c>
+      <c r="C73" s="80">
+        <v>1</v>
+      </c>
+      <c r="D73" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="F73" s="88" t="s">
+      <c r="F73" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="G73" s="107"/>
+      <c r="G73" s="106"/>
       <c r="H73" s="29"/>
       <c r="I73" s="29"/>
       <c r="J73" s="29"/>
@@ -11977,26 +12055,28 @@
       <c r="Q73" s="29"/>
       <c r="R73" s="29"/>
       <c r="S73" s="29"/>
-      <c r="T73" s="120"/>
+      <c r="T73" s="119"/>
     </row>
     <row r="74" spans="1:20" ht="29.45" thickBot="1">
       <c r="A74" s="23">
         <v>1</v>
       </c>
-      <c r="B74" s="77"/>
+      <c r="B74" s="126">
+        <v>3</v>
+      </c>
       <c r="C74" s="24">
         <v>1</v>
       </c>
       <c r="D74" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E74" s="78" t="s">
+      <c r="E74" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="F74" s="86" t="s">
+      <c r="F74" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="G74" s="113">
+      <c r="G74" s="112">
         <v>11111</v>
       </c>
       <c r="H74" s="29"/>
@@ -12011,7 +12091,7 @@
       <c r="Q74" s="29"/>
       <c r="R74" s="29"/>
       <c r="S74" s="29"/>
-      <c r="T74" s="120"/>
+      <c r="T74" s="119"/>
     </row>
     <row r="75" spans="1:20">
       <c r="A75" s="30"/>
@@ -12020,7 +12100,7 @@
       <c r="D75" s="29"/>
       <c r="E75" s="34"/>
       <c r="F75" s="29"/>
-      <c r="G75" s="124"/>
+      <c r="G75" s="123"/>
       <c r="H75" s="29"/>
       <c r="I75" s="29"/>
       <c r="J75" s="29"/>
@@ -12033,7 +12113,7 @@
       <c r="Q75" s="29"/>
       <c r="R75" s="29"/>
       <c r="S75" s="29"/>
-      <c r="T75" s="120"/>
+      <c r="T75" s="119"/>
     </row>
     <row r="76" spans="1:20">
       <c r="A76" s="30"/>
@@ -12042,7 +12122,7 @@
       <c r="D76" s="29"/>
       <c r="E76" s="29"/>
       <c r="F76" s="29"/>
-      <c r="G76" s="124"/>
+      <c r="G76" s="123"/>
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
       <c r="J76" s="29"/>
@@ -12055,7 +12135,7 @@
       <c r="Q76" s="29"/>
       <c r="R76" s="29"/>
       <c r="S76" s="29"/>
-      <c r="T76" s="120"/>
+      <c r="T76" s="119"/>
     </row>
     <row r="77" spans="1:20" ht="57.95">
       <c r="A77" s="30"/>
@@ -12064,7 +12144,7 @@
       <c r="D77" s="29"/>
       <c r="E77" s="29"/>
       <c r="F77" s="29"/>
-      <c r="G77" s="124"/>
+      <c r="G77" s="123"/>
       <c r="H77" s="29">
         <v>14</v>
       </c>
@@ -12085,7 +12165,7 @@
       <c r="Q77" s="29"/>
       <c r="R77" s="29"/>
       <c r="S77" s="29"/>
-      <c r="T77" s="120"/>
+      <c r="T77" s="119"/>
     </row>
     <row r="78" spans="1:20" ht="57.95">
       <c r="A78" s="30"/>
@@ -12094,7 +12174,7 @@
       <c r="D78" s="29"/>
       <c r="E78" s="29"/>
       <c r="F78" s="29"/>
-      <c r="G78" s="124"/>
+      <c r="G78" s="123"/>
       <c r="H78" s="29">
         <v>15</v>
       </c>
@@ -12115,7 +12195,7 @@
       <c r="Q78" s="29"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29"/>
-      <c r="T78" s="120"/>
+      <c r="T78" s="119"/>
     </row>
     <row r="79" spans="1:20" ht="57.95">
       <c r="A79" s="30"/>
@@ -12124,7 +12204,7 @@
       <c r="D79" s="29"/>
       <c r="E79" s="29"/>
       <c r="F79" s="29"/>
-      <c r="G79" s="124"/>
+      <c r="G79" s="123"/>
       <c r="H79" s="29">
         <v>16</v>
       </c>
@@ -12145,7 +12225,7 @@
       <c r="Q79" s="29"/>
       <c r="R79" s="29"/>
       <c r="S79" s="29"/>
-      <c r="T79" s="120"/>
+      <c r="T79" s="119"/>
     </row>
     <row r="80" spans="1:20" ht="57.95">
       <c r="A80" s="30"/>
@@ -12154,7 +12234,7 @@
       <c r="D80" s="29"/>
       <c r="E80" s="29"/>
       <c r="F80" s="29"/>
-      <c r="G80" s="124"/>
+      <c r="G80" s="123"/>
       <c r="H80" s="29">
         <v>17</v>
       </c>
@@ -12175,7 +12255,7 @@
       <c r="Q80" s="29"/>
       <c r="R80" s="29"/>
       <c r="S80" s="29"/>
-      <c r="T80" s="120"/>
+      <c r="T80" s="119"/>
     </row>
     <row r="81" spans="1:20">
       <c r="A81" s="30"/>
@@ -12184,7 +12264,7 @@
       <c r="D81" s="29"/>
       <c r="E81" s="29"/>
       <c r="F81" s="29"/>
-      <c r="G81" s="124"/>
+      <c r="G81" s="123"/>
       <c r="H81" s="29"/>
       <c r="I81" s="29"/>
       <c r="J81" s="29"/>
@@ -12197,7 +12277,7 @@
       <c r="Q81" s="29"/>
       <c r="R81" s="29"/>
       <c r="S81" s="29"/>
-      <c r="T81" s="120"/>
+      <c r="T81" s="119"/>
     </row>
     <row r="82" spans="1:20">
       <c r="A82" s="30"/>
@@ -12206,7 +12286,7 @@
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
       <c r="F82" s="29"/>
-      <c r="G82" s="124"/>
+      <c r="G82" s="123"/>
       <c r="H82" s="29"/>
       <c r="I82" s="29"/>
       <c r="J82" s="29"/>
@@ -12219,7 +12299,7 @@
       <c r="Q82" s="29"/>
       <c r="R82" s="29"/>
       <c r="S82" s="29"/>
-      <c r="T82" s="120"/>
+      <c r="T82" s="119"/>
     </row>
     <row r="83" spans="1:20">
       <c r="A83" s="30"/>
@@ -12228,7 +12308,7 @@
       <c r="D83" s="29"/>
       <c r="E83" s="29"/>
       <c r="F83" s="29"/>
-      <c r="G83" s="124"/>
+      <c r="G83" s="123"/>
       <c r="H83" s="29"/>
       <c r="I83" s="29"/>
       <c r="J83" s="29"/>
@@ -12241,7 +12321,7 @@
       <c r="Q83" s="29"/>
       <c r="R83" s="29"/>
       <c r="S83" s="29"/>
-      <c r="T83" s="120"/>
+      <c r="T83" s="119"/>
     </row>
     <row r="84" spans="1:20" ht="15" thickBot="1">
       <c r="A84" s="30"/>
@@ -12250,7 +12330,7 @@
       <c r="D84" s="29"/>
       <c r="E84" s="29"/>
       <c r="F84" s="29"/>
-      <c r="G84" s="124"/>
+      <c r="G84" s="123"/>
       <c r="H84" s="29"/>
       <c r="I84" s="29"/>
       <c r="J84" s="29"/>
@@ -12263,7 +12343,7 @@
       <c r="Q84" s="29"/>
       <c r="R84" s="29"/>
       <c r="S84" s="29"/>
-      <c r="T84" s="120"/>
+      <c r="T84" s="119"/>
     </row>
     <row r="85" spans="1:20" ht="72.599999999999994">
       <c r="A85" s="5">
@@ -12284,7 +12364,7 @@
       <c r="F85" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G85" s="104"/>
+      <c r="G85" s="103"/>
       <c r="H85" s="29">
         <v>18</v>
       </c>
@@ -12313,7 +12393,7 @@
       <c r="S85" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T85" s="120">
+      <c r="T85" s="119">
         <v>1</v>
       </c>
     </row>
@@ -12333,10 +12413,10 @@
       <c r="E86" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F86" s="90" t="s">
+      <c r="F86" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G86" s="108"/>
+      <c r="G86" s="107"/>
       <c r="H86" s="29"/>
       <c r="I86" s="29"/>
       <c r="J86" s="29"/>
@@ -12349,20 +12429,26 @@
       <c r="Q86" s="29"/>
       <c r="R86" s="29"/>
       <c r="S86" s="29"/>
-      <c r="T86" s="120"/>
+      <c r="T86" s="119"/>
     </row>
     <row r="87" spans="1:20">
-      <c r="A87" s="6"/>
+      <c r="A87" s="6">
+        <v>3</v>
+      </c>
       <c r="B87" s="7"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
+      <c r="C87" s="8">
+        <v>1</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E87" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F87" s="90" t="s">
+      <c r="F87" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="G87" s="108"/>
+      <c r="G87" s="107"/>
       <c r="H87" s="29"/>
       <c r="I87" s="29"/>
       <c r="J87" s="29"/>
@@ -12375,28 +12461,28 @@
       <c r="Q87" s="29"/>
       <c r="R87" s="29"/>
       <c r="S87" s="29"/>
-      <c r="T87" s="120"/>
+      <c r="T87" s="119"/>
     </row>
     <row r="88" spans="1:20" ht="15" thickBot="1">
-      <c r="A88" s="82">
-        <v>3</v>
-      </c>
-      <c r="B88" s="83">
-        <v>2</v>
-      </c>
-      <c r="C88" s="81">
-        <v>1</v>
-      </c>
-      <c r="D88" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E88" s="81" t="s">
+      <c r="A88" s="81">
+        <v>4</v>
+      </c>
+      <c r="B88" s="82">
+        <v>2</v>
+      </c>
+      <c r="C88" s="80">
+        <v>1</v>
+      </c>
+      <c r="D88" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E88" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="F88" s="88" t="s">
+      <c r="F88" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="G88" s="107"/>
+      <c r="G88" s="106"/>
       <c r="H88" s="29"/>
       <c r="I88" s="29"/>
       <c r="J88" s="29"/>
@@ -12409,26 +12495,28 @@
       <c r="Q88" s="29"/>
       <c r="R88" s="29"/>
       <c r="S88" s="29"/>
-      <c r="T88" s="120"/>
+      <c r="T88" s="119"/>
     </row>
     <row r="89" spans="1:20" ht="29.1">
-      <c r="A89" s="79">
-        <v>1</v>
-      </c>
-      <c r="B89" s="32"/>
+      <c r="A89" s="78">
+        <v>1</v>
+      </c>
+      <c r="B89" s="127">
+        <v>3</v>
+      </c>
       <c r="C89" s="28">
         <v>1</v>
       </c>
       <c r="D89" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E89" s="80" t="s">
+      <c r="E89" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F89" s="87" t="s">
+      <c r="F89" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="G89" s="99">
+      <c r="G89" s="98">
         <v>11111</v>
       </c>
       <c r="H89" s="29"/>
@@ -12443,13 +12531,15 @@
       <c r="Q89" s="29"/>
       <c r="R89" s="29"/>
       <c r="S89" s="29"/>
-      <c r="T89" s="120"/>
+      <c r="T89" s="119"/>
     </row>
     <row r="90" spans="1:20" ht="29.45" thickBot="1">
       <c r="A90" s="13">
         <v>2</v>
       </c>
-      <c r="B90" s="14"/>
+      <c r="B90" s="128">
+        <v>3</v>
+      </c>
       <c r="C90" s="15">
         <v>2</v>
       </c>
@@ -12462,7 +12552,7 @@
       <c r="F90" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="G90" s="100">
+      <c r="G90" s="99">
         <v>14111</v>
       </c>
       <c r="H90" s="29"/>
@@ -12477,7 +12567,7 @@
       <c r="Q90" s="29"/>
       <c r="R90" s="29"/>
       <c r="S90" s="29"/>
-      <c r="T90" s="120"/>
+      <c r="T90" s="119"/>
     </row>
     <row r="91" spans="1:20">
       <c r="A91" s="30"/>
@@ -12486,7 +12576,7 @@
       <c r="D91" s="29"/>
       <c r="E91" s="29"/>
       <c r="F91" s="29"/>
-      <c r="G91" s="124"/>
+      <c r="G91" s="123"/>
       <c r="H91" s="29"/>
       <c r="I91" s="29"/>
       <c r="J91" s="29"/>
@@ -12499,7 +12589,7 @@
       <c r="Q91" s="29"/>
       <c r="R91" s="29"/>
       <c r="S91" s="29"/>
-      <c r="T91" s="120"/>
+      <c r="T91" s="119"/>
     </row>
     <row r="92" spans="1:20" ht="44.1" thickBot="1">
       <c r="A92" s="30"/>
@@ -12508,7 +12598,7 @@
       <c r="D92" s="29"/>
       <c r="E92" s="29"/>
       <c r="F92" s="29"/>
-      <c r="G92" s="124"/>
+      <c r="G92" s="123"/>
       <c r="H92" s="29">
         <v>19</v>
       </c>
@@ -12529,7 +12619,7 @@
       <c r="Q92" s="29"/>
       <c r="R92" s="29"/>
       <c r="S92" s="29"/>
-      <c r="T92" s="120"/>
+      <c r="T92" s="119"/>
     </row>
     <row r="93" spans="1:20" ht="72.599999999999994">
       <c r="A93" s="5">
@@ -12550,7 +12640,7 @@
       <c r="F93" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G93" s="104"/>
+      <c r="G93" s="103"/>
       <c r="H93" s="29">
         <v>19</v>
       </c>
@@ -12579,7 +12669,7 @@
       <c r="S93" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T93" s="120">
+      <c r="T93" s="119">
         <v>1</v>
       </c>
     </row>
@@ -12599,10 +12689,10 @@
       <c r="E94" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F94" s="90" t="s">
+      <c r="F94" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G94" s="108"/>
+      <c r="G94" s="107"/>
       <c r="H94" s="29"/>
       <c r="I94" s="29"/>
       <c r="J94" s="29"/>
@@ -12615,20 +12705,26 @@
       <c r="Q94" s="29"/>
       <c r="R94" s="29"/>
       <c r="S94" s="29"/>
-      <c r="T94" s="120"/>
+      <c r="T94" s="119"/>
     </row>
     <row r="95" spans="1:20">
-      <c r="A95" s="6"/>
+      <c r="A95" s="6">
+        <v>3</v>
+      </c>
       <c r="B95" s="7"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
+      <c r="C95" s="8">
+        <v>1</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E95" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F95" s="90" t="s">
+      <c r="F95" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="G95" s="108"/>
+      <c r="G95" s="107"/>
       <c r="H95" s="29"/>
       <c r="I95" s="29"/>
       <c r="J95" s="29"/>
@@ -12641,28 +12737,28 @@
       <c r="Q95" s="29"/>
       <c r="R95" s="29"/>
       <c r="S95" s="29"/>
-      <c r="T95" s="120"/>
+      <c r="T95" s="119"/>
     </row>
     <row r="96" spans="1:20" ht="15" thickBot="1">
-      <c r="A96" s="82">
-        <v>3</v>
-      </c>
-      <c r="B96" s="83">
-        <v>2</v>
-      </c>
-      <c r="C96" s="81">
-        <v>1</v>
-      </c>
-      <c r="D96" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E96" s="81" t="s">
+      <c r="A96" s="81">
+        <v>4</v>
+      </c>
+      <c r="B96" s="82">
+        <v>2</v>
+      </c>
+      <c r="C96" s="80">
+        <v>1</v>
+      </c>
+      <c r="D96" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E96" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="F96" s="88" t="s">
+      <c r="F96" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="G96" s="107"/>
+      <c r="G96" s="106"/>
       <c r="H96" s="29"/>
       <c r="I96" s="29"/>
       <c r="J96" s="29"/>
@@ -12675,26 +12771,28 @@
       <c r="Q96" s="29"/>
       <c r="R96" s="29"/>
       <c r="S96" s="29"/>
-      <c r="T96" s="120"/>
+      <c r="T96" s="119"/>
     </row>
     <row r="97" spans="1:21" ht="29.1">
-      <c r="A97" s="79">
-        <v>1</v>
-      </c>
-      <c r="B97" s="32"/>
+      <c r="A97" s="78">
+        <v>1</v>
+      </c>
+      <c r="B97" s="127">
+        <v>3</v>
+      </c>
       <c r="C97" s="28">
         <v>1</v>
       </c>
       <c r="D97" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E97" s="80" t="s">
+      <c r="E97" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F97" s="87" t="s">
+      <c r="F97" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="G97" s="99">
+      <c r="G97" s="98">
         <v>11111</v>
       </c>
       <c r="H97" s="29"/>
@@ -12709,13 +12807,15 @@
       <c r="Q97" s="29"/>
       <c r="R97" s="29"/>
       <c r="S97" s="29"/>
-      <c r="T97" s="120"/>
+      <c r="T97" s="119"/>
     </row>
     <row r="98" spans="1:21" ht="29.45" thickBot="1">
       <c r="A98" s="13">
         <v>2</v>
       </c>
-      <c r="B98" s="14"/>
+      <c r="B98" s="128">
+        <v>3</v>
+      </c>
       <c r="C98" s="15">
         <v>2</v>
       </c>
@@ -12728,7 +12828,7 @@
       <c r="F98" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="G98" s="100">
+      <c r="G98" s="99">
         <v>14111</v>
       </c>
       <c r="H98" s="29"/>
@@ -12743,7 +12843,7 @@
       <c r="Q98" s="29"/>
       <c r="R98" s="29"/>
       <c r="S98" s="29"/>
-      <c r="T98" s="120"/>
+      <c r="T98" s="119"/>
     </row>
     <row r="99" spans="1:21">
       <c r="A99" s="30"/>
@@ -12752,7 +12852,7 @@
       <c r="D99" s="29"/>
       <c r="E99" s="29"/>
       <c r="F99" s="29"/>
-      <c r="G99" s="124"/>
+      <c r="G99" s="123"/>
       <c r="H99" s="29"/>
       <c r="I99" s="29"/>
       <c r="J99" s="29"/>
@@ -12765,7 +12865,7 @@
       <c r="Q99" s="29"/>
       <c r="R99" s="29"/>
       <c r="S99" s="29"/>
-      <c r="T99" s="120"/>
+      <c r="T99" s="119"/>
     </row>
     <row r="100" spans="1:21">
       <c r="A100" s="30"/>
@@ -12774,7 +12874,7 @@
       <c r="D100" s="29"/>
       <c r="E100" s="29"/>
       <c r="F100" s="29"/>
-      <c r="G100" s="124"/>
+      <c r="G100" s="123"/>
       <c r="H100" s="29"/>
       <c r="I100" s="29"/>
       <c r="J100" s="29"/>
@@ -12787,7 +12887,7 @@
       <c r="Q100" s="29"/>
       <c r="R100" s="29"/>
       <c r="S100" s="29"/>
-      <c r="T100" s="120"/>
+      <c r="T100" s="119"/>
     </row>
     <row r="101" spans="1:21" ht="43.5">
       <c r="A101" s="30"/>
@@ -12796,7 +12896,7 @@
       <c r="D101" s="29"/>
       <c r="E101" s="29"/>
       <c r="F101" s="29"/>
-      <c r="G101" s="124"/>
+      <c r="G101" s="123"/>
       <c r="H101" s="29">
         <v>20</v>
       </c>
@@ -12817,7 +12917,7 @@
       <c r="Q101" s="29"/>
       <c r="R101" s="29"/>
       <c r="S101" s="29"/>
-      <c r="T101" s="120"/>
+      <c r="T101" s="119"/>
     </row>
     <row r="102" spans="1:21" ht="15" thickBot="1">
       <c r="A102" s="30"/>
@@ -12826,7 +12926,7 @@
       <c r="D102" s="29"/>
       <c r="E102" s="29"/>
       <c r="F102" s="29"/>
-      <c r="G102" s="124"/>
+      <c r="G102" s="123"/>
       <c r="H102" s="29"/>
       <c r="I102" s="29"/>
       <c r="J102" s="29"/>
@@ -12839,7 +12939,7 @@
       <c r="Q102" s="29"/>
       <c r="R102" s="29"/>
       <c r="S102" s="29"/>
-      <c r="T102" s="120"/>
+      <c r="T102" s="119"/>
     </row>
     <row r="103" spans="1:21" ht="72.599999999999994">
       <c r="A103" s="5">
@@ -12860,7 +12960,7 @@
       <c r="F103" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G103" s="104"/>
+      <c r="G103" s="103"/>
       <c r="H103" s="29">
         <v>20</v>
       </c>
@@ -12889,7 +12989,7 @@
       <c r="S103" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="T103" s="120">
+      <c r="T103" s="119">
         <v>1</v>
       </c>
     </row>
@@ -12909,10 +13009,10 @@
       <c r="E104" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F104" s="90" t="s">
+      <c r="F104" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G104" s="108"/>
+      <c r="G104" s="107"/>
       <c r="H104" s="29"/>
       <c r="I104" s="29"/>
       <c r="J104" s="29"/>
@@ -12925,20 +13025,26 @@
       <c r="Q104" s="29"/>
       <c r="R104" s="29"/>
       <c r="S104" s="29"/>
-      <c r="T104" s="120"/>
+      <c r="T104" s="119"/>
     </row>
     <row r="105" spans="1:21">
-      <c r="A105" s="6"/>
-      <c r="B105" s="7"/>
+      <c r="A105" s="6">
+        <v>3</v>
+      </c>
+      <c r="B105" s="7">
+        <v>2</v>
+      </c>
       <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
+      <c r="D105" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E105" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F105" s="90" t="s">
+      <c r="F105" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="G105" s="108"/>
+      <c r="G105" s="107"/>
       <c r="H105" s="29"/>
       <c r="I105" s="29"/>
       <c r="J105" s="29"/>
@@ -12951,28 +13057,28 @@
       <c r="Q105" s="29"/>
       <c r="R105" s="29"/>
       <c r="S105" s="29"/>
-      <c r="T105" s="120"/>
+      <c r="T105" s="119"/>
     </row>
     <row r="106" spans="1:21" ht="15" thickBot="1">
-      <c r="A106" s="82">
-        <v>3</v>
-      </c>
-      <c r="B106" s="83">
-        <v>2</v>
-      </c>
-      <c r="C106" s="81">
-        <v>1</v>
-      </c>
-      <c r="D106" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E106" s="81" t="s">
+      <c r="A106" s="81">
+        <v>4</v>
+      </c>
+      <c r="B106" s="82">
+        <v>2</v>
+      </c>
+      <c r="C106" s="80">
+        <v>1</v>
+      </c>
+      <c r="D106" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E106" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="F106" s="88" t="s">
+      <c r="F106" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="G106" s="107"/>
+      <c r="G106" s="106"/>
       <c r="H106" s="29"/>
       <c r="I106" s="29"/>
       <c r="J106" s="29"/>
@@ -12985,26 +13091,28 @@
       <c r="Q106" s="29"/>
       <c r="R106" s="29"/>
       <c r="S106" s="29"/>
-      <c r="T106" s="120"/>
+      <c r="T106" s="119"/>
     </row>
     <row r="107" spans="1:21" ht="29.1">
-      <c r="A107" s="79">
-        <v>1</v>
-      </c>
-      <c r="B107" s="32"/>
+      <c r="A107" s="78">
+        <v>1</v>
+      </c>
+      <c r="B107" s="127">
+        <v>3</v>
+      </c>
       <c r="C107" s="28">
         <v>1</v>
       </c>
       <c r="D107" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E107" s="80" t="s">
+      <c r="E107" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F107" s="87" t="s">
+      <c r="F107" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="G107" s="99">
+      <c r="G107" s="98">
         <v>11111</v>
       </c>
       <c r="H107" s="29"/>
@@ -13019,13 +13127,15 @@
       <c r="Q107" s="29"/>
       <c r="R107" s="29"/>
       <c r="S107" s="29"/>
-      <c r="T107" s="120"/>
+      <c r="T107" s="119"/>
     </row>
     <row r="108" spans="1:21" ht="29.45" thickBot="1">
       <c r="A108" s="13">
         <v>2</v>
       </c>
-      <c r="B108" s="14"/>
+      <c r="B108" s="128">
+        <v>3</v>
+      </c>
       <c r="C108" s="15">
         <v>2</v>
       </c>
@@ -13038,7 +13148,7 @@
       <c r="F108" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="G108" s="100">
+      <c r="G108" s="99">
         <v>14111</v>
       </c>
       <c r="H108" s="29"/>
@@ -13053,7 +13163,7 @@
       <c r="Q108" s="29"/>
       <c r="R108" s="29"/>
       <c r="S108" s="29"/>
-      <c r="T108" s="120"/>
+      <c r="T108" s="119"/>
     </row>
     <row r="109" spans="1:21">
       <c r="A109" s="30"/>
@@ -13062,7 +13172,7 @@
       <c r="D109" s="29"/>
       <c r="E109" s="34"/>
       <c r="F109" s="29"/>
-      <c r="G109" s="124"/>
+      <c r="G109" s="123"/>
       <c r="H109" s="29"/>
       <c r="I109" s="29"/>
       <c r="J109" s="29"/>
@@ -13075,7 +13185,7 @@
       <c r="Q109" s="33"/>
       <c r="R109" s="29"/>
       <c r="S109" s="29"/>
-      <c r="T109" s="121"/>
+      <c r="T109" s="120"/>
       <c r="U109" s="29"/>
     </row>
     <row r="110" spans="1:21">
@@ -13085,7 +13195,7 @@
       <c r="D110" s="29"/>
       <c r="E110" s="34"/>
       <c r="F110" s="29"/>
-      <c r="G110" s="124"/>
+      <c r="G110" s="123"/>
       <c r="H110" s="29"/>
       <c r="I110" s="29"/>
       <c r="J110" s="29"/>
@@ -13098,7 +13208,7 @@
       <c r="Q110" s="33"/>
       <c r="R110" s="29"/>
       <c r="S110" s="29"/>
-      <c r="T110" s="121"/>
+      <c r="T110" s="120"/>
       <c r="U110" s="29"/>
     </row>
     <row r="111" spans="1:21" ht="87.6" thickBot="1">
@@ -13108,7 +13218,7 @@
       <c r="D111" s="22"/>
       <c r="E111" s="22"/>
       <c r="F111" s="22"/>
-      <c r="G111" s="126"/>
+      <c r="G111" s="125"/>
       <c r="H111" s="22">
         <v>100</v>
       </c>
@@ -13117,7 +13227,7 @@
         <v>113</v>
       </c>
       <c r="K111" s="22"/>
-      <c r="L111" s="84" t="s">
+      <c r="L111" s="83" t="s">
         <v>114</v>
       </c>
       <c r="M111" s="22"/>
@@ -13127,7 +13237,7 @@
       <c r="Q111" s="22"/>
       <c r="R111" s="22"/>
       <c r="S111" s="22"/>
-      <c r="T111" s="122"/>
+      <c r="T111" s="121"/>
     </row>
     <row r="112" spans="1:21">
       <c r="M112" s="29"/>

</xml_diff>